<commit_message>
updating college and withdrawals issues
</commit_message>
<xml_diff>
--- a/python/Inputs/Inputs.xlsx
+++ b/python/Inputs/Inputs.xlsx
@@ -1,41 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rthor\Dropbox\PC\Desktop\Projects\personalFinances\python\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F48873E-1E07-4C2C-A9BD-E779AEE6B091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E4CF37-82D5-48B0-89C3-957D1C961B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="786" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
     <sheet name="Salary" sheetId="20" r:id="rId2"/>
-    <sheet name="Salary (Past)" sheetId="26" r:id="rId3"/>
+    <sheet name="Social Security" sheetId="26" r:id="rId3"/>
     <sheet name="Accounts" sheetId="4" r:id="rId4"/>
     <sheet name="Allocations" sheetId="2" r:id="rId5"/>
     <sheet name="Earnings" sheetId="3" r:id="rId6"/>
     <sheet name="Loans" sheetId="21" r:id="rId7"/>
-    <sheet name="MONTHLY" sheetId="22" r:id="rId8"/>
-    <sheet name="Home" sheetId="6" r:id="rId9"/>
-    <sheet name="Rent" sheetId="7" r:id="rId10"/>
-    <sheet name="Car" sheetId="5" r:id="rId11"/>
-    <sheet name="Food" sheetId="8" r:id="rId12"/>
-    <sheet name="Shopping" sheetId="23" r:id="rId13"/>
-    <sheet name="Activities" sheetId="24" r:id="rId14"/>
-    <sheet name="Subscriptions" sheetId="11" r:id="rId15"/>
-    <sheet name="Personal Care" sheetId="10" r:id="rId16"/>
-    <sheet name="Gifts" sheetId="13" r:id="rId17"/>
-    <sheet name="Health Care" sheetId="9" r:id="rId18"/>
-    <sheet name="Pet" sheetId="12" r:id="rId19"/>
-    <sheet name="Education" sheetId="15" r:id="rId20"/>
-    <sheet name="Vacation" sheetId="16" r:id="rId21"/>
-    <sheet name="Major" sheetId="25" r:id="rId22"/>
-    <sheet name="Random" sheetId="18" r:id="rId23"/>
+    <sheet name="Home" sheetId="6" r:id="rId8"/>
+    <sheet name="Rent" sheetId="7" r:id="rId9"/>
+    <sheet name="Car" sheetId="5" r:id="rId10"/>
+    <sheet name="Food" sheetId="8" r:id="rId11"/>
+    <sheet name="Shopping" sheetId="23" r:id="rId12"/>
+    <sheet name="Activities" sheetId="24" r:id="rId13"/>
+    <sheet name="Subscriptions" sheetId="11" r:id="rId14"/>
+    <sheet name="Personal Care" sheetId="10" r:id="rId15"/>
+    <sheet name="Gifts" sheetId="13" r:id="rId16"/>
+    <sheet name="Health Care" sheetId="9" r:id="rId17"/>
+    <sheet name="Pet" sheetId="12" r:id="rId18"/>
+    <sheet name="Education" sheetId="15" r:id="rId19"/>
+    <sheet name="Vacation" sheetId="16" r:id="rId20"/>
+    <sheet name="Major" sheetId="25" r:id="rId21"/>
+    <sheet name="Random" sheetId="18" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="166">
   <si>
     <t>Years</t>
   </si>
@@ -406,9 +405,6 @@
   </si>
   <si>
     <t>etfFund</t>
-  </si>
-  <si>
-    <t>Home Chef</t>
   </si>
   <si>
     <t>% salary</t>
@@ -1374,10 +1370,10 @@
     <xf numFmtId="165" fontId="0" fillId="34" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="20" fillId="35" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="20" fillId="35" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1446,9 +1442,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1486,7 +1482,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1592,7 +1588,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1734,7 +1730,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1747,8 +1743,8 @@
   </sheetPr>
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:G16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1774,7 +1770,7 @@
       </c>
       <c r="B2" s="48"/>
       <c r="C2" s="44">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1783,7 +1779,7 @@
       </c>
       <c r="B3" s="48"/>
       <c r="C3" s="44">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D3" s="20"/>
     </row>
@@ -1794,10 +1790,10 @@
       </c>
       <c r="B5" s="48"/>
       <c r="C5" s="44">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" s="17">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -1844,7 +1840,7 @@
     </row>
     <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" s="48"/>
       <c r="C8" s="44">
@@ -1924,14 +1920,14 @@
     <row r="13" spans="1:13" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="67" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D14" s="68" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1940,7 +1936,7 @@
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="12">
-        <v>119800</v>
+        <v>132000</v>
       </c>
       <c r="D15" s="18">
         <v>111435</v>
@@ -1967,22 +1963,22 @@
         <v>42</v>
       </c>
       <c r="C17" s="4">
-        <v>0.02</v>
+        <v>-0.02</v>
       </c>
       <c r="D17" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F17" s="61">
+        <v>0.03</v>
+      </c>
+      <c r="G17" s="61">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="E17" s="4">
+      <c r="H17" s="61">
         <v>0.05</v>
-      </c>
-      <c r="F17" s="61">
-        <v>-0.02</v>
-      </c>
-      <c r="G17" s="61">
-        <v>0.01</v>
-      </c>
-      <c r="H17" s="61">
-        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1993,10 +1989,10 @@
         <v>42</v>
       </c>
       <c r="C18" s="4">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D18" s="4">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="E18" s="4">
         <v>0.05</v>
@@ -2008,7 +2004,7 @@
       </c>
       <c r="B19" s="48"/>
       <c r="C19" s="7">
-        <v>0.25</v>
+        <v>0.33</v>
       </c>
       <c r="D19" s="53"/>
       <c r="E19" s="10"/>
@@ -2019,7 +2015,7 @@
       </c>
       <c r="B20" s="48"/>
       <c r="C20" s="44">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D20" s="53"/>
       <c r="E20" s="10"/>
@@ -2032,13 +2028,13 @@
         <v>42</v>
       </c>
       <c r="C21" s="4">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="D21" s="4">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="E21" s="4">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="22" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -2048,7 +2044,7 @@
       </c>
       <c r="B23" s="48"/>
       <c r="C23" s="4">
-        <v>3.5000000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="D23" s="54">
         <v>3.5000000000000003E-2</v>
@@ -2061,7 +2057,7 @@
       </c>
       <c r="B24" s="48"/>
       <c r="C24" s="4">
-        <v>2.3E-2</v>
+        <v>0</v>
       </c>
       <c r="D24" s="54">
         <v>2.3E-2</v>
@@ -2418,216 +2414,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF624D77-2870-4555-B62D-733EBDFE0F64}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:Z16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11" customWidth="1"/>
-    <col min="5" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" style="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" style="28"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I1"/>
-      <c r="M1"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="I2"/>
-      <c r="M2"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="12">
-        <v>2200</v>
-      </c>
-      <c r="I3"/>
-      <c r="M3"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="18">
-        <v>75</v>
-      </c>
-      <c r="D4" s="41">
-        <v>50</v>
-      </c>
-      <c r="E4" s="41">
-        <v>25</v>
-      </c>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="41"/>
-      <c r="T4" s="41"/>
-      <c r="U4" s="41"/>
-      <c r="V4" s="41"/>
-      <c r="W4" s="41"/>
-      <c r="X4" s="41"/>
-      <c r="Y4" s="41"/>
-      <c r="Z4" s="41"/>
-    </row>
-    <row r="5" spans="1:26" s="70" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="C5" s="70" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" s="70" t="s">
-        <v>131</v>
-      </c>
-      <c r="E5" s="70" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="12">
-        <v>25</v>
-      </c>
-      <c r="D6" s="12">
-        <v>50</v>
-      </c>
-      <c r="E6" s="12">
-        <v>100</v>
-      </c>
-      <c r="I6"/>
-      <c r="M6"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="12">
-        <v>20</v>
-      </c>
-      <c r="I7"/>
-      <c r="M7"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I8"/>
-      <c r="M8"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="12">
-        <v>150</v>
-      </c>
-      <c r="I9"/>
-      <c r="M9"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="12">
-        <v>20</v>
-      </c>
-      <c r="I10"/>
-      <c r="M10"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="12">
-        <v>40</v>
-      </c>
-      <c r="I11"/>
-      <c r="M11"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="39"/>
-      <c r="I12"/>
-      <c r="M12"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="I13"/>
-      <c r="M13"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I14"/>
-      <c r="M14"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I15"/>
-      <c r="M15"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I16"/>
-      <c r="M16"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1794CECF-4906-4EF5-BFE7-0830CAF2B342}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -2706,7 +2492,7 @@
       </c>
       <c r="B3" s="19">
         <f ca="1">A3+RANDBETWEEN(5,9)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3" s="18">
         <v>23500</v>
@@ -2776,11 +2562,11 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="17">
         <f ca="1">IF(B3&lt;Inputs!$C$3,B3,"")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="18">
         <v>30000</v>
@@ -2818,36 +2604,36 @@
       </c>
       <c r="B6" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" s="18">
         <v>30000</v>
       </c>
       <c r="D6" s="33">
-        <f t="shared" ref="D6:D20" si="1">IF(ISNUMBER(C6),20%,"")</f>
+        <f t="shared" ref="D6:D19" si="1">IF(ISNUMBER(C6),20%,"")</f>
         <v>0.2</v>
       </c>
       <c r="E6" s="33">
-        <f t="shared" ref="E6:E20" si="2">IF(ISNUMBER(D6),-15%,"")</f>
+        <f t="shared" ref="E6:E19" si="2">IF(ISNUMBER(D6),-15%,"")</f>
         <v>-0.15</v>
       </c>
       <c r="F6" s="60">
-        <f t="shared" ref="F6:F20" si="3">IF(ISNUMBER(E6),5,"")</f>
+        <f t="shared" ref="F6:F19" si="3">IF(ISNUMBER(E6),5,"")</f>
         <v>5</v>
       </c>
       <c r="G6" s="37">
-        <f t="shared" ref="G6:G20" si="4">IF(ISNUMBER(F6),1.9%,"")</f>
+        <f t="shared" ref="G6:G19" si="4">IF(ISNUMBER(F6),1.9%,"")</f>
         <v>1.9E-2</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <f ca="1">IF(B5&lt;Inputs!$C$3,B5,"")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="18">
         <v>35000</v>
@@ -2872,17 +2658,17 @@
         <v>44</v>
       </c>
       <c r="J7" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <f ca="1">IF(B6&lt;Inputs!$C$3,B6,"")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" s="18">
         <v>22500</v>
@@ -2907,11 +2693,11 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <f ca="1">IF(B7&lt;Inputs!$C$3,B7,"")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C9" s="18">
         <v>40000</v>
@@ -2936,11 +2722,11 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="17">
         <f ca="1">IF(B8&lt;Inputs!$C$3,B8,"")</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C10" s="18">
         <v>22500</v>
@@ -2965,15 +2751,15 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
         <f ca="1">IF(B9&lt;Inputs!$C$3,B9,"")</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B11" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C11" s="18">
         <f ca="1">IF(ISNUMBER(B11),RANDBETWEEN(40000,60000),"")</f>
-        <v>41547</v>
+        <v>48978</v>
       </c>
       <c r="D11" s="33">
         <f t="shared" ca="1" si="1"/>
@@ -2995,15 +2781,15 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
         <f ca="1">IF(B10&lt;Inputs!$C$3,B10,"")</f>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B12" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" s="18">
-        <f t="shared" ref="C12:C20" ca="1" si="5">IF(ISNUMBER(B12),RANDBETWEEN(40000,60000),"")</f>
-        <v>42002</v>
+        <f t="shared" ref="C12:C19" ca="1" si="5">IF(ISNUMBER(B12),RANDBETWEEN(40000,60000),"")</f>
+        <v>57637</v>
       </c>
       <c r="D12" s="33">
         <f t="shared" ca="1" si="1"/>
@@ -3025,15 +2811,15 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <f ca="1">IF(B11&lt;Inputs!$C$3,B11,"")</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B13" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C13" s="18">
         <f t="shared" ca="1" si="5"/>
-        <v>49575</v>
+        <v>50463</v>
       </c>
       <c r="D13" s="33">
         <f t="shared" ca="1" si="1"/>
@@ -3055,15 +2841,15 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <f ca="1">IF(B12&lt;Inputs!$C$3,B12,"")</f>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14" s="19">
-        <f t="shared" ref="B14:B20" ca="1" si="6">IF(ISNUMBER(A14),A14+RANDBETWEEN(5,9),"")</f>
-        <v>41</v>
+        <f t="shared" ref="B14:B19" ca="1" si="6">IF(ISNUMBER(A14),A14+RANDBETWEEN(5,9),"")</f>
+        <v>46</v>
       </c>
       <c r="C14" s="18">
         <f t="shared" ca="1" si="5"/>
-        <v>56767</v>
+        <v>42871</v>
       </c>
       <c r="D14" s="33">
         <f t="shared" ca="1" si="1"/>
@@ -3085,15 +2871,15 @@
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
         <f ca="1">IF(B13&lt;Inputs!$C$3,B13,"")</f>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B15" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C15" s="18">
         <f t="shared" ca="1" si="5"/>
-        <v>57451</v>
+        <v>58428</v>
       </c>
       <c r="D15" s="33">
         <f t="shared" ca="1" si="1"/>
@@ -3113,243 +2899,243 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="17">
+      <c r="A16" s="17" t="str">
         <f ca="1">IF(B14&lt;Inputs!$C$3,B14,"")</f>
-        <v>41</v>
-      </c>
-      <c r="B16" s="19">
+        <v/>
+      </c>
+      <c r="B16" s="19" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
-      </c>
-      <c r="C16" s="18">
+        <v/>
+      </c>
+      <c r="C16" s="18" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>46464</v>
-      </c>
-      <c r="D16" s="33">
+        <v/>
+      </c>
+      <c r="D16" s="33" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="E16" s="33">
+        <v/>
+      </c>
+      <c r="E16" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.15</v>
-      </c>
-      <c r="F16" s="60">
+        <v/>
+      </c>
+      <c r="F16" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="G16" s="37">
+        <v/>
+      </c>
+      <c r="G16" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9E-2</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="17">
+      <c r="A17" s="17" t="str">
         <f ca="1">IF(B15&lt;Inputs!$C$3,B15,"")</f>
-        <v>42</v>
-      </c>
-      <c r="B17" s="19">
+        <v/>
+      </c>
+      <c r="B17" s="19" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>48</v>
-      </c>
-      <c r="C17" s="18">
+        <v/>
+      </c>
+      <c r="C17" s="18" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>44549</v>
-      </c>
-      <c r="D17" s="33">
+        <v/>
+      </c>
+      <c r="D17" s="33" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="E17" s="33">
+        <v/>
+      </c>
+      <c r="E17" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.15</v>
-      </c>
-      <c r="F17" s="60">
+        <v/>
+      </c>
+      <c r="F17" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="G17" s="37">
+        <v/>
+      </c>
+      <c r="G17" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9E-2</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="17">
+      <c r="A18" s="17" t="str">
         <f ca="1">IF(B16&lt;Inputs!$C$3,B16,"")</f>
-        <v>46</v>
-      </c>
-      <c r="B18" s="19">
+        <v/>
+      </c>
+      <c r="B18" s="19" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>51</v>
-      </c>
-      <c r="C18" s="18">
+        <v/>
+      </c>
+      <c r="C18" s="18" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>52366</v>
-      </c>
-      <c r="D18" s="33">
+        <v/>
+      </c>
+      <c r="D18" s="33" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="E18" s="33">
+        <v/>
+      </c>
+      <c r="E18" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.15</v>
-      </c>
-      <c r="F18" s="60">
+        <v/>
+      </c>
+      <c r="F18" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="G18" s="37">
+        <v/>
+      </c>
+      <c r="G18" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9E-2</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="17">
+      <c r="A19" s="17" t="str">
         <f ca="1">IF(B17&lt;Inputs!$C$3,B17,"")</f>
-        <v>48</v>
-      </c>
-      <c r="B19" s="19">
+        <v/>
+      </c>
+      <c r="B19" s="19" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>54</v>
-      </c>
-      <c r="C19" s="18">
+        <v/>
+      </c>
+      <c r="C19" s="18" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>53833</v>
-      </c>
-      <c r="D19" s="33">
+        <v/>
+      </c>
+      <c r="D19" s="33" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="E19" s="33">
+        <v/>
+      </c>
+      <c r="E19" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.15</v>
-      </c>
-      <c r="F19" s="60">
+        <v/>
+      </c>
+      <c r="F19" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="G19" s="37">
+        <v/>
+      </c>
+      <c r="G19" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9E-2</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="17">
+      <c r="A20" s="17" t="str">
         <f ca="1">IF(B18&lt;Inputs!$C$3,B18,"")</f>
-        <v>51</v>
-      </c>
-      <c r="B20" s="19">
-        <f t="shared" ref="B20:B24" ca="1" si="7">IF(ISNUMBER(A20),A20+RANDBETWEEN(5,9),"")</f>
-        <v>59</v>
-      </c>
-      <c r="C20" s="18">
-        <f t="shared" ref="C20:C24" ca="1" si="8">IF(ISNUMBER(B20),RANDBETWEEN(40000,60000),"")</f>
-        <v>40143</v>
-      </c>
-      <c r="D20" s="33">
-        <f t="shared" ref="D20:D24" ca="1" si="9">IF(ISNUMBER(C20),20%,"")</f>
-        <v>0.2</v>
-      </c>
-      <c r="E20" s="33">
-        <f t="shared" ref="E20:E24" ca="1" si="10">IF(ISNUMBER(D20),-15%,"")</f>
-        <v>-0.15</v>
-      </c>
-      <c r="F20" s="60">
-        <f t="shared" ref="F20:F24" ca="1" si="11">IF(ISNUMBER(E20),5,"")</f>
-        <v>5</v>
-      </c>
-      <c r="G20" s="37">
-        <f t="shared" ref="G20:G24" ca="1" si="12">IF(ISNUMBER(F20),1.9%,"")</f>
-        <v>1.9E-2</v>
+        <v/>
+      </c>
+      <c r="B20" s="19" t="str">
+        <f t="shared" ref="B20:B25" ca="1" si="7">IF(ISNUMBER(A20),A20+RANDBETWEEN(5,9),"")</f>
+        <v/>
+      </c>
+      <c r="C20" s="18" t="str">
+        <f t="shared" ref="C20:C25" ca="1" si="8">IF(ISNUMBER(B20),RANDBETWEEN(40000,60000),"")</f>
+        <v/>
+      </c>
+      <c r="D20" s="33" t="str">
+        <f t="shared" ref="D20:D25" ca="1" si="9">IF(ISNUMBER(C20),20%,"")</f>
+        <v/>
+      </c>
+      <c r="E20" s="33" t="str">
+        <f t="shared" ref="E20:E25" ca="1" si="10">IF(ISNUMBER(D20),-15%,"")</f>
+        <v/>
+      </c>
+      <c r="F20" s="60" t="str">
+        <f t="shared" ref="F20:F25" ca="1" si="11">IF(ISNUMBER(E20),5,"")</f>
+        <v/>
+      </c>
+      <c r="G20" s="37" t="str">
+        <f t="shared" ref="G20:G25" ca="1" si="12">IF(ISNUMBER(F20),1.9%,"")</f>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="17">
+      <c r="A21" s="17" t="str">
         <f ca="1">IF(B19&lt;Inputs!$C$3,B19,"")</f>
-        <v>54</v>
-      </c>
-      <c r="B21" s="19">
+        <v/>
+      </c>
+      <c r="B21" s="19" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>59</v>
-      </c>
-      <c r="C21" s="18">
+        <v/>
+      </c>
+      <c r="C21" s="18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>53714</v>
-      </c>
-      <c r="D21" s="33">
+        <v/>
+      </c>
+      <c r="D21" s="33" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.2</v>
-      </c>
-      <c r="E21" s="33">
+        <v/>
+      </c>
+      <c r="E21" s="33" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>-0.15</v>
-      </c>
-      <c r="F21" s="60">
+        <v/>
+      </c>
+      <c r="F21" s="60" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>5</v>
-      </c>
-      <c r="G21" s="37">
+        <v/>
+      </c>
+      <c r="G21" s="37" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>1.9E-2</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="17">
+      <c r="A22" s="17" t="str">
         <f ca="1">IF(B20&lt;Inputs!$C$3,B20,"")</f>
-        <v>59</v>
-      </c>
-      <c r="B22" s="19">
+        <v/>
+      </c>
+      <c r="B22" s="19" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>68</v>
-      </c>
-      <c r="C22" s="18">
+        <v/>
+      </c>
+      <c r="C22" s="18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>44191</v>
-      </c>
-      <c r="D22" s="33">
+        <v/>
+      </c>
+      <c r="D22" s="33" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.2</v>
-      </c>
-      <c r="E22" s="33">
+        <v/>
+      </c>
+      <c r="E22" s="33" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>-0.15</v>
-      </c>
-      <c r="F22" s="60">
+        <v/>
+      </c>
+      <c r="F22" s="60" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>5</v>
-      </c>
-      <c r="G22" s="37">
+        <v/>
+      </c>
+      <c r="G22" s="37" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>1.9E-2</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="17">
+      <c r="A23" s="17" t="str">
         <f ca="1">IF(B21&lt;Inputs!$C$3,B21,"")</f>
-        <v>59</v>
-      </c>
-      <c r="B23" s="19">
+        <v/>
+      </c>
+      <c r="B23" s="19" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>67</v>
-      </c>
-      <c r="C23" s="18">
+        <v/>
+      </c>
+      <c r="C23" s="18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>53250</v>
-      </c>
-      <c r="D23" s="33">
+        <v/>
+      </c>
+      <c r="D23" s="33" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.2</v>
-      </c>
-      <c r="E23" s="33">
+        <v/>
+      </c>
+      <c r="E23" s="33" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>-0.15</v>
-      </c>
-      <c r="F23" s="60">
+        <v/>
+      </c>
+      <c r="F23" s="60" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>5</v>
-      </c>
-      <c r="G23" s="37">
+        <v/>
+      </c>
+      <c r="G23" s="37" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>1.9E-2</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -3388,27 +3174,27 @@
         <v/>
       </c>
       <c r="B25" s="19" t="str">
-        <f t="shared" ref="B25" ca="1" si="13">IF(ISNUMBER(A25),A25+RANDBETWEEN(5,9),"")</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="C25" s="18" t="str">
-        <f t="shared" ref="C25" ca="1" si="14">IF(ISNUMBER(B25),RANDBETWEEN(40000,60000),"")</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="D25" s="33" t="str">
-        <f t="shared" ref="D25" ca="1" si="15">IF(ISNUMBER(C25),20%,"")</f>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="E25" s="33" t="str">
-        <f t="shared" ref="E25" ca="1" si="16">IF(ISNUMBER(D25),-15%,"")</f>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="F25" s="60" t="str">
-        <f t="shared" ref="F25" ca="1" si="17">IF(ISNUMBER(E25),5,"")</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="G25" s="37" t="str">
-        <f t="shared" ref="G25" ca="1" si="18">IF(ISNUMBER(F25),1.9%,"")</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
     </row>
@@ -3418,7 +3204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676B8487-6DFC-49C1-8D36-5F31E0BAAB85}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -3426,7 +3212,7 @@
   <dimension ref="A2:M100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3450,13 +3236,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="12">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="E2" s="31" t="s">
         <v>44</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -3467,7 +3253,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="12">
-        <v>200</v>
+        <v>350</v>
       </c>
       <c r="E3" s="28"/>
     </row>
@@ -3484,15 +3270,9 @@
       <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="57" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="58">
-        <v>200</v>
-      </c>
+      <c r="A5" s="57"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="58"/>
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -3979,7 +3759,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC9F971-9022-47EF-A46E-8DC0E4F5AA23}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -3997,7 +3777,7 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2" s="48" t="s">
         <v>3</v>
@@ -4009,12 +3789,12 @@
         <v>44</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="57" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>3</v>
@@ -4026,7 +3806,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="57" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>3</v>
@@ -4038,7 +3818,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B5" s="48" t="s">
         <v>3</v>
@@ -4050,7 +3830,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="57" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6" s="48" t="s">
         <v>3</v>
@@ -4062,7 +3842,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B7" s="48" t="s">
         <v>3</v>
@@ -4074,7 +3854,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="57" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B8" s="48" t="s">
         <v>3</v>
@@ -4550,7 +4330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE44382-030D-4D66-91A6-AD13ADE699AE}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -4558,7 +4338,7 @@
   <dimension ref="A2:F100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4568,42 +4348,42 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2" s="48" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="12">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E2" s="31" t="s">
         <v>44</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="12">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E4" s="28"/>
     </row>
@@ -5097,7 +4877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819F17BD-3D74-4EC4-8440-AE3BD931E3E0}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -5112,10 +4892,10 @@
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="9.77734375" customWidth="1"/>
-    <col min="9" max="9" width="9.77734375" style="30" customWidth="1"/>
-    <col min="10" max="12" width="9.77734375" customWidth="1"/>
-    <col min="13" max="13" width="9.77734375" style="28" customWidth="1"/>
+    <col min="3" max="8" width="9.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="30" customWidth="1"/>
+    <col min="10" max="12" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -5144,7 +4924,7 @@
     </row>
     <row r="4" spans="1:13" s="41" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>3</v>
@@ -5214,7 +4994,7 @@
         <v>44</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="43" t="s">
         <v>56</v>
@@ -5234,7 +5014,7 @@
         <v>57</v>
       </c>
       <c r="D9" s="43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E9" s="43"/>
     </row>
@@ -5244,7 +5024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B80A56B-A8E7-4876-AA03-58B13EB97F16}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -5252,7 +5032,7 @@
   <dimension ref="A2:M102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5283,7 +5063,7 @@
         <v>44</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -5300,7 +5080,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>3</v>
@@ -5318,7 +5098,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="12">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="E5" s="28"/>
     </row>
@@ -5827,7 +5607,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB74594-BD38-45FF-80A6-CFC24DC4475F}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -5835,7 +5615,7 @@
   <dimension ref="A2:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="C5:F5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5854,7 +5634,7 @@
         <v>88</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" s="4">
         <v>0.01</v>
@@ -5864,7 +5644,7 @@
     <row r="3" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>80</v>
@@ -5884,7 +5664,7 @@
     </row>
     <row r="5" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" s="48" t="s">
         <v>80</v>
@@ -5904,16 +5684,16 @@
     </row>
     <row r="6" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C6" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="E6" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="F6" s="43" t="s">
         <v>140</v>
-      </c>
-      <c r="F6" s="43" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -5921,7 +5701,7 @@
         <v>44</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E7" s="28"/>
     </row>
@@ -5931,7 +5711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9619A95F-7E98-400F-8F9A-C5237BD03C09}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -5939,7 +5719,7 @@
   <dimension ref="A2:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5957,13 +5737,13 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" s="48" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="12">
-        <v>1500</v>
+        <v>150</v>
       </c>
       <c r="D2" s="45"/>
     </row>
@@ -5975,7 +5755,7 @@
         <v>50</v>
       </c>
       <c r="C3" s="12">
-        <v>3200</v>
+        <v>3250</v>
       </c>
       <c r="D3" s="45"/>
       <c r="E3" s="28"/>
@@ -5986,7 +5766,7 @@
       </c>
       <c r="B4" s="48"/>
       <c r="C4" s="7">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D4" s="46"/>
       <c r="E4" s="28"/>
@@ -5999,7 +5779,7 @@
         <v>50</v>
       </c>
       <c r="C5" s="12">
-        <v>9200</v>
+        <v>9800</v>
       </c>
       <c r="D5" s="45"/>
       <c r="E5" s="28"/>
@@ -6020,10 +5800,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="44">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E7" s="44">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -6074,7 +5854,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B12" s="48" t="s">
         <v>80</v>
@@ -6093,7 +5873,7 @@
         <v>44</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E14" s="28"/>
     </row>
@@ -6103,7 +5883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9EC8FB3-02FD-435D-B914-7C2BC091879C}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -6111,7 +5891,7 @@
   <dimension ref="A2:M102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6135,13 +5915,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="12">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="E2" s="31" t="s">
         <v>44</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -6674,672 +6454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7356A922-E8A8-48FA-A1B5-573C5ADA2096}">
-  <sheetPr>
-    <tabColor theme="4" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:C100"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:B30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.109375" style="63"/>
-    <col min="2" max="2" width="11.5546875" style="65" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="65"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="5"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="62">
-        <v>0</v>
-      </c>
-      <c r="B2" s="12">
-        <v>0</v>
-      </c>
-      <c r="C2" s="18"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="66">
-        <f>A2+1</f>
-        <v>1</v>
-      </c>
-      <c r="B3" s="64">
-        <v>0</v>
-      </c>
-      <c r="C3" s="64"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="66">
-        <f t="shared" ref="A4:A26" si="0">A3+1</f>
-        <v>2</v>
-      </c>
-      <c r="B4" s="64">
-        <v>0</v>
-      </c>
-      <c r="C4" s="64"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="66">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B5" s="64">
-        <v>0</v>
-      </c>
-      <c r="C5" s="64"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="66">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B6" s="64">
-        <v>70000</v>
-      </c>
-      <c r="C6" s="64"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="66">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B7" s="64">
-        <v>75000</v>
-      </c>
-      <c r="C7" s="64"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="66">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B8" s="64">
-        <v>80000</v>
-      </c>
-      <c r="C8" s="64"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="66">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B9" s="64">
-        <v>85000</v>
-      </c>
-      <c r="C9" s="64"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="66">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B10" s="64">
-        <v>90000</v>
-      </c>
-      <c r="C10" s="64"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="66">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B11" s="64">
-        <v>95000</v>
-      </c>
-      <c r="C11" s="64"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="66">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B12" s="64">
-        <v>400000</v>
-      </c>
-      <c r="C12" s="64"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="66">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B13" s="64">
-        <f ca="1">(1+(RANDBETWEEN(2,10)/100))*B12</f>
-        <v>408000</v>
-      </c>
-      <c r="C13" s="64"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="66">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B14" s="64">
-        <f t="shared" ref="B14:B26" ca="1" si="1">(1+(RANDBETWEEN(2,10)/100))*B13</f>
-        <v>436560</v>
-      </c>
-      <c r="C14" s="64"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="66">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B15" s="64">
-        <f t="shared" ca="1" si="1"/>
-        <v>480216.00000000006</v>
-      </c>
-      <c r="C15" s="64"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="66">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B16" s="64">
-        <f t="shared" ca="1" si="1"/>
-        <v>489820.32000000007</v>
-      </c>
-      <c r="C16" s="64"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="66">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B17" s="64">
-        <f t="shared" ca="1" si="1"/>
-        <v>533904.14880000008</v>
-      </c>
-      <c r="C17" s="64"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="66">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B18" s="64">
-        <f t="shared" ca="1" si="1"/>
-        <v>555260.31475200015</v>
-      </c>
-      <c r="C18" s="64"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="66">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B19" s="64">
-        <f t="shared" ca="1" si="1"/>
-        <v>577470.72734208021</v>
-      </c>
-      <c r="C19" s="64"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="66">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B20" s="64">
-        <f t="shared" ca="1" si="1"/>
-        <v>629443.09280286753</v>
-      </c>
-      <c r="C20" s="64"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="66">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B21" s="64">
-        <f t="shared" ca="1" si="1"/>
-        <v>667209.67837103957</v>
-      </c>
-      <c r="C21" s="64"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="66">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B22" s="64">
-        <f t="shared" ca="1" si="1"/>
-        <v>693898.06550588121</v>
-      </c>
-      <c r="C22" s="64"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="66">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B23" s="64">
-        <f t="shared" ca="1" si="1"/>
-        <v>742470.93009129295</v>
-      </c>
-      <c r="C23" s="64"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="66">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B24" s="64">
-        <f t="shared" ca="1" si="1"/>
-        <v>772169.76729494473</v>
-      </c>
-      <c r="C24" s="64"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="66">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B25" s="64">
-        <f t="shared" ca="1" si="1"/>
-        <v>795334.86031379306</v>
-      </c>
-      <c r="C25" s="64"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="66">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B26" s="64">
-        <f t="shared" ca="1" si="1"/>
-        <v>874868.3463451725</v>
-      </c>
-      <c r="C26" s="64"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="66"/>
-      <c r="B27" s="64"/>
-      <c r="C27" s="64"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="66"/>
-      <c r="B28" s="64"/>
-      <c r="C28" s="64"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="66"/>
-      <c r="B29" s="64"/>
-      <c r="C29" s="64"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="66"/>
-      <c r="B30" s="64"/>
-      <c r="C30" s="64"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="66"/>
-      <c r="B31" s="64"/>
-      <c r="C31" s="64"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="66"/>
-      <c r="B32" s="64"/>
-      <c r="C32" s="64"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="66"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="64"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="66"/>
-      <c r="B34" s="64"/>
-      <c r="C34" s="64"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="66"/>
-      <c r="B35" s="64"/>
-      <c r="C35" s="64"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="66"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="64"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="66"/>
-      <c r="B37" s="64"/>
-      <c r="C37" s="64"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="66"/>
-      <c r="B38" s="64"/>
-      <c r="C38" s="64"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="66"/>
-      <c r="B39" s="64"/>
-      <c r="C39" s="64"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="66"/>
-      <c r="B40" s="64"/>
-      <c r="C40" s="64"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="66"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="64"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="66"/>
-      <c r="B42" s="64"/>
-      <c r="C42" s="64"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="66"/>
-      <c r="B43" s="64"/>
-      <c r="C43" s="64"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="66"/>
-      <c r="B44" s="64"/>
-      <c r="C44" s="64"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="66"/>
-      <c r="B45" s="64"/>
-      <c r="C45" s="64"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="66"/>
-      <c r="B46" s="64"/>
-      <c r="C46" s="64"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="66"/>
-      <c r="B47" s="64"/>
-      <c r="C47" s="64"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="66"/>
-      <c r="B48" s="64"/>
-      <c r="C48" s="64"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="66"/>
-      <c r="B49" s="64"/>
-      <c r="C49" s="64"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="66"/>
-      <c r="B50" s="64"/>
-      <c r="C50" s="64"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="66"/>
-      <c r="B51" s="64"/>
-      <c r="C51" s="64"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="66"/>
-      <c r="B52" s="64"/>
-      <c r="C52" s="64"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="66"/>
-      <c r="B53" s="64"/>
-      <c r="C53" s="64"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="66"/>
-      <c r="B54" s="64"/>
-      <c r="C54" s="64"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="66"/>
-      <c r="B55" s="64"/>
-      <c r="C55" s="64"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="66"/>
-      <c r="B56" s="64"/>
-      <c r="C56" s="64"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="66"/>
-      <c r="B57" s="64"/>
-      <c r="C57" s="64"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="66"/>
-      <c r="B58" s="64"/>
-      <c r="C58" s="64"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="66"/>
-      <c r="B59" s="64"/>
-      <c r="C59" s="64"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="66"/>
-      <c r="B60" s="64"/>
-      <c r="C60" s="64"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="66"/>
-      <c r="B61" s="64"/>
-      <c r="C61" s="64"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="66"/>
-      <c r="B62" s="64"/>
-      <c r="C62" s="64"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="66"/>
-      <c r="B63" s="64"/>
-      <c r="C63" s="64"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="66"/>
-      <c r="B64" s="64"/>
-      <c r="C64" s="64"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="66"/>
-      <c r="B65" s="64"/>
-      <c r="C65" s="64"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="66"/>
-      <c r="B66" s="64"/>
-      <c r="C66" s="64"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="66"/>
-      <c r="B67" s="64"/>
-      <c r="C67" s="64"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="66"/>
-      <c r="B68" s="64"/>
-      <c r="C68" s="64"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="66"/>
-      <c r="B69" s="64"/>
-      <c r="C69" s="64"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="66"/>
-      <c r="B70" s="64"/>
-      <c r="C70" s="64"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="66"/>
-      <c r="B71" s="64"/>
-      <c r="C71" s="64"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="66"/>
-      <c r="B72" s="64"/>
-      <c r="C72" s="64"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="66"/>
-      <c r="B73" s="64"/>
-      <c r="C73" s="64"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="66"/>
-      <c r="B74" s="64"/>
-      <c r="C74" s="64"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="66"/>
-      <c r="B75" s="64"/>
-      <c r="C75" s="64"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="66"/>
-      <c r="B76" s="64"/>
-      <c r="C76" s="64"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="66"/>
-      <c r="B77" s="64"/>
-      <c r="C77" s="64"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="66"/>
-      <c r="B78" s="64"/>
-      <c r="C78" s="64"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="66"/>
-      <c r="B79" s="64"/>
-      <c r="C79" s="64"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="66"/>
-      <c r="B80" s="64"/>
-      <c r="C80" s="64"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="66"/>
-      <c r="B81" s="64"/>
-      <c r="C81" s="64"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="66"/>
-      <c r="B82" s="64"/>
-      <c r="C82" s="64"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="66"/>
-      <c r="B83" s="64"/>
-      <c r="C83" s="64"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="66"/>
-      <c r="B84" s="64"/>
-      <c r="C84" s="64"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="66"/>
-      <c r="B85" s="64"/>
-      <c r="C85" s="64"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="66"/>
-      <c r="B86" s="64"/>
-      <c r="C86" s="64"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="66"/>
-      <c r="B87" s="64"/>
-      <c r="C87" s="64"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="66"/>
-      <c r="B88" s="64"/>
-      <c r="C88" s="64"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="66"/>
-      <c r="B89" s="64"/>
-      <c r="C89" s="64"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" s="66"/>
-      <c r="B90" s="64"/>
-      <c r="C90" s="64"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="66"/>
-      <c r="B91" s="64"/>
-      <c r="C91" s="64"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" s="66"/>
-      <c r="B92" s="64"/>
-      <c r="C92" s="64"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="66"/>
-      <c r="B93" s="64"/>
-      <c r="C93" s="64"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="66"/>
-      <c r="B94" s="64"/>
-      <c r="C94" s="64"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="66"/>
-      <c r="B95" s="64"/>
-      <c r="C95" s="64"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="66"/>
-      <c r="B96" s="64"/>
-      <c r="C96" s="64"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="66"/>
-      <c r="B97" s="64"/>
-      <c r="C97" s="64"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="66"/>
-      <c r="B98" s="64"/>
-      <c r="C98" s="64"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="66"/>
-      <c r="B99" s="64"/>
-      <c r="C99" s="64"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="66"/>
-      <c r="B100" s="64"/>
-      <c r="C100" s="64"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D15979-A930-400D-9247-8AA007EF54B0}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -7441,7 +6556,672 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7356A922-E8A8-48FA-A1B5-573C5ADA2096}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:C100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" style="63"/>
+    <col min="2" max="2" width="11.5546875" style="65" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="65"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="62">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12">
+        <v>0</v>
+      </c>
+      <c r="C2" s="18"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="66">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="64">
+        <v>0</v>
+      </c>
+      <c r="C3" s="64"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="66">
+        <f t="shared" ref="A4:A26" si="0">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="64">
+        <v>0</v>
+      </c>
+      <c r="C4" s="64"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="66">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="64">
+        <v>0</v>
+      </c>
+      <c r="C5" s="64"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="66">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="64">
+        <v>70000</v>
+      </c>
+      <c r="C6" s="64"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="66">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="64">
+        <v>75000</v>
+      </c>
+      <c r="C7" s="64"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="66">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="64">
+        <v>80000</v>
+      </c>
+      <c r="C8" s="64"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="66">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="64">
+        <v>85000</v>
+      </c>
+      <c r="C9" s="64"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="66">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="64">
+        <v>90000</v>
+      </c>
+      <c r="C10" s="64"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="66">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="64">
+        <v>95000</v>
+      </c>
+      <c r="C11" s="64"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="66">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="64">
+        <v>400000</v>
+      </c>
+      <c r="C12" s="64"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="66">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="64">
+        <f ca="1">(1+(RANDBETWEEN(2,10)/100))*B12</f>
+        <v>436000.00000000006</v>
+      </c>
+      <c r="C13" s="64"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="66">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="64">
+        <f t="shared" ref="B14:B26" ca="1" si="1">(1+(RANDBETWEEN(2,10)/100))*B13</f>
+        <v>457800.00000000006</v>
+      </c>
+      <c r="C14" s="64"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="66">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="64">
+        <f t="shared" ca="1" si="1"/>
+        <v>480690.00000000006</v>
+      </c>
+      <c r="C15" s="64"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="66">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="64">
+        <f t="shared" ca="1" si="1"/>
+        <v>528759.00000000012</v>
+      </c>
+      <c r="C16" s="64"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="66">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="64">
+        <f t="shared" ca="1" si="1"/>
+        <v>565772.13000000012</v>
+      </c>
+      <c r="C17" s="64"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="66">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="64">
+        <f t="shared" ca="1" si="1"/>
+        <v>605376.17910000018</v>
+      </c>
+      <c r="C18" s="64"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="66">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="64">
+        <f t="shared" ca="1" si="1"/>
+        <v>653806.27342800028</v>
+      </c>
+      <c r="C19" s="64"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="66">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="64">
+        <f t="shared" ca="1" si="1"/>
+        <v>666882.39889656031</v>
+      </c>
+      <c r="C20" s="64"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="66">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="64">
+        <f t="shared" ca="1" si="1"/>
+        <v>686888.87086345709</v>
+      </c>
+      <c r="C21" s="64"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="66">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="64">
+        <f t="shared" ca="1" si="1"/>
+        <v>721233.31440663</v>
+      </c>
+      <c r="C22" s="64"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="66">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="64">
+        <f t="shared" ca="1" si="1"/>
+        <v>757294.98012696148</v>
+      </c>
+      <c r="C23" s="64"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="66">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="64">
+        <f t="shared" ca="1" si="1"/>
+        <v>817878.5785371185</v>
+      </c>
+      <c r="C24" s="64"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="66">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="64">
+        <f t="shared" ca="1" si="1"/>
+        <v>899666.43639083044</v>
+      </c>
+      <c r="C25" s="64"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="66">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="64">
+        <f t="shared" ca="1" si="1"/>
+        <v>953646.4225742803</v>
+      </c>
+      <c r="C26" s="64"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="66"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="64"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="66"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="64"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="66"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="66"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="64"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="66"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="66"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="66"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="66"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="64"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="66"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="64"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="66"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="64"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="66"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="64"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="66"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="64"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="66"/>
+      <c r="B39" s="64"/>
+      <c r="C39" s="64"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="66"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="64"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="66"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="64"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="66"/>
+      <c r="B42" s="64"/>
+      <c r="C42" s="64"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="66"/>
+      <c r="B43" s="64"/>
+      <c r="C43" s="64"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="66"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="64"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="66"/>
+      <c r="B45" s="64"/>
+      <c r="C45" s="64"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="66"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="64"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="66"/>
+      <c r="B47" s="64"/>
+      <c r="C47" s="64"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="66"/>
+      <c r="B48" s="64"/>
+      <c r="C48" s="64"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="66"/>
+      <c r="B49" s="64"/>
+      <c r="C49" s="64"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="66"/>
+      <c r="B50" s="64"/>
+      <c r="C50" s="64"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="66"/>
+      <c r="B51" s="64"/>
+      <c r="C51" s="64"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="66"/>
+      <c r="B52" s="64"/>
+      <c r="C52" s="64"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="66"/>
+      <c r="B53" s="64"/>
+      <c r="C53" s="64"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="66"/>
+      <c r="B54" s="64"/>
+      <c r="C54" s="64"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="66"/>
+      <c r="B55" s="64"/>
+      <c r="C55" s="64"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="66"/>
+      <c r="B56" s="64"/>
+      <c r="C56" s="64"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="66"/>
+      <c r="B57" s="64"/>
+      <c r="C57" s="64"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="66"/>
+      <c r="B58" s="64"/>
+      <c r="C58" s="64"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="66"/>
+      <c r="B59" s="64"/>
+      <c r="C59" s="64"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="66"/>
+      <c r="B60" s="64"/>
+      <c r="C60" s="64"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="66"/>
+      <c r="B61" s="64"/>
+      <c r="C61" s="64"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="66"/>
+      <c r="B62" s="64"/>
+      <c r="C62" s="64"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="66"/>
+      <c r="B63" s="64"/>
+      <c r="C63" s="64"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="66"/>
+      <c r="B64" s="64"/>
+      <c r="C64" s="64"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="66"/>
+      <c r="B65" s="64"/>
+      <c r="C65" s="64"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="66"/>
+      <c r="B66" s="64"/>
+      <c r="C66" s="64"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="66"/>
+      <c r="B67" s="64"/>
+      <c r="C67" s="64"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="66"/>
+      <c r="B68" s="64"/>
+      <c r="C68" s="64"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="66"/>
+      <c r="B69" s="64"/>
+      <c r="C69" s="64"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="66"/>
+      <c r="B70" s="64"/>
+      <c r="C70" s="64"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="66"/>
+      <c r="B71" s="64"/>
+      <c r="C71" s="64"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="66"/>
+      <c r="B72" s="64"/>
+      <c r="C72" s="64"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="66"/>
+      <c r="B73" s="64"/>
+      <c r="C73" s="64"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="66"/>
+      <c r="B74" s="64"/>
+      <c r="C74" s="64"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="66"/>
+      <c r="B75" s="64"/>
+      <c r="C75" s="64"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="66"/>
+      <c r="B76" s="64"/>
+      <c r="C76" s="64"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="66"/>
+      <c r="B77" s="64"/>
+      <c r="C77" s="64"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="66"/>
+      <c r="B78" s="64"/>
+      <c r="C78" s="64"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="66"/>
+      <c r="B79" s="64"/>
+      <c r="C79" s="64"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="66"/>
+      <c r="B80" s="64"/>
+      <c r="C80" s="64"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="66"/>
+      <c r="B81" s="64"/>
+      <c r="C81" s="64"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="66"/>
+      <c r="B82" s="64"/>
+      <c r="C82" s="64"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="66"/>
+      <c r="B83" s="64"/>
+      <c r="C83" s="64"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="66"/>
+      <c r="B84" s="64"/>
+      <c r="C84" s="64"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="66"/>
+      <c r="B85" s="64"/>
+      <c r="C85" s="64"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="66"/>
+      <c r="B86" s="64"/>
+      <c r="C86" s="64"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="66"/>
+      <c r="B87" s="64"/>
+      <c r="C87" s="64"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="66"/>
+      <c r="B88" s="64"/>
+      <c r="C88" s="64"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="66"/>
+      <c r="B89" s="64"/>
+      <c r="C89" s="64"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="66"/>
+      <c r="B90" s="64"/>
+      <c r="C90" s="64"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="66"/>
+      <c r="B91" s="64"/>
+      <c r="C91" s="64"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="66"/>
+      <c r="B92" s="64"/>
+      <c r="C92" s="64"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="66"/>
+      <c r="B93" s="64"/>
+      <c r="C93" s="64"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="66"/>
+      <c r="B94" s="64"/>
+      <c r="C94" s="64"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="66"/>
+      <c r="B95" s="64"/>
+      <c r="C95" s="64"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="66"/>
+      <c r="B96" s="64"/>
+      <c r="C96" s="64"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="66"/>
+      <c r="B97" s="64"/>
+      <c r="C97" s="64"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="66"/>
+      <c r="B98" s="64"/>
+      <c r="C98" s="64"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="66"/>
+      <c r="B99" s="64"/>
+      <c r="C99" s="64"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="66"/>
+      <c r="B100" s="64"/>
+      <c r="C100" s="64"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A3623E-739B-4E92-BD1F-A85E8AE93729}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -7449,7 +7229,7 @@
   <dimension ref="A2:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7560,7 +7340,7 @@
         <v>44</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E10" s="28"/>
     </row>
@@ -7570,7 +7350,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952CE758-0D5B-42FD-99EA-05A20ACE7083}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -7578,7 +7358,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7616,13 +7396,13 @@
         <v>34</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>44</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -7649,7 +7429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E24977A-EA5F-4BA3-9B84-B620814A1B9D}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -7704,7 +7484,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" s="28"/>
     </row>
@@ -7722,7 +7502,7 @@
   <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7736,7 +7516,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C1" s="5"/>
     </row>
@@ -7793,7 +7573,7 @@
         <v>-1</v>
       </c>
       <c r="B6" s="41">
-        <v>119800</v>
+        <v>124403</v>
       </c>
       <c r="C6" s="41">
         <v>100000</v>
@@ -8281,8 +8061,8 @@
   </sheetPr>
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8298,7 +8078,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="76" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="13" t="s">
@@ -8308,12 +8088,12 @@
       <c r="D1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="75"/>
+      <c r="A2" s="76"/>
       <c r="B2" s="21" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>27</v>
@@ -8322,13 +8102,13 @@
         <v>28</v>
       </c>
       <c r="F2" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="G2" s="72" t="s">
+      <c r="H2" s="21" t="s">
         <v>134</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -8336,7 +8116,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="25">
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="C3" s="65" t="s">
         <v>101</v>
@@ -8345,7 +8125,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F3" s="73"/>
       <c r="G3" s="41"/>
@@ -8359,7 +8139,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="25">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="C4" s="65" t="s">
         <v>101</v>
@@ -8384,10 +8164,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="25">
-        <v>3500</v>
+        <v>30000</v>
       </c>
       <c r="C5" s="65" t="s">
         <v>101</v>
@@ -8407,7 +8187,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="25">
-        <v>3500</v>
+        <v>16000</v>
       </c>
       <c r="C6" s="65" t="s">
         <v>101</v>
@@ -8435,7 +8215,7 @@
         <v>116</v>
       </c>
       <c r="B7" s="25">
-        <v>6000</v>
+        <v>14000</v>
       </c>
       <c r="C7" s="65" t="s">
         <v>101</v>
@@ -8460,13 +8240,14 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B8" s="25">
-        <v>80000</v>
+        <f>130000-B9</f>
+        <v>85000</v>
       </c>
       <c r="C8" s="65" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>31</v>
@@ -8480,13 +8261,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B9" s="25">
-        <v>15000</v>
+        <v>45000</v>
       </c>
       <c r="C9" s="65" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>30</v>
@@ -8500,13 +8281,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B10" s="25">
-        <v>55000</v>
+        <v>75000</v>
       </c>
       <c r="C10" s="65" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>31</v>
@@ -8520,13 +8301,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B11" s="25">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="C11" s="65" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>30</v>
@@ -8543,7 +8324,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="25">
-        <v>7500</v>
+        <v>14000</v>
       </c>
       <c r="C12" s="65" t="s">
         <v>101</v>
@@ -8566,10 +8347,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B13" s="25">
-        <v>90000</v>
+        <v>70000</v>
       </c>
       <c r="C13" s="65" t="s">
         <v>101</v>
@@ -9141,7 +8922,7 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView zoomScale="84" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:F10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9302,10 +9083,10 @@
       <c r="D8" s="36">
         <v>0</v>
       </c>
-      <c r="E8" s="76">
+      <c r="E8" s="75">
         <v>0</v>
       </c>
-      <c r="F8" s="76">
+      <c r="F8" s="75">
         <v>0</v>
       </c>
     </row>
@@ -9344,10 +9125,10 @@
       <c r="D10" s="36">
         <v>0</v>
       </c>
-      <c r="E10" s="76">
+      <c r="E10" s="75">
         <v>0</v>
       </c>
-      <c r="F10" s="76">
+      <c r="F10" s="75">
         <v>0</v>
       </c>
     </row>
@@ -9859,7 +9640,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="76" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="13" t="s">
@@ -9870,7 +9651,7 @@
       <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="75"/>
+      <c r="A2" s="76"/>
       <c r="B2" s="21" t="s">
         <v>16</v>
       </c>
@@ -10096,10 +9877,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>37</v>
@@ -10111,7 +9892,7 @@
         <v>44</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -10744,23 +10525,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5E4A8C-AC10-43B6-BDCF-45FA095A9419}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C228208F-908D-44CE-BB18-24656B27C42F}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -10768,7 +10532,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10837,7 +10601,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="17">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="B3" s="19">
         <v>17</v>
@@ -10849,7 +10613,7 @@
         <v>0.2</v>
       </c>
       <c r="E3" s="4">
-        <v>1.4999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F3" s="8">
         <v>30</v>
@@ -10867,7 +10631,7 @@
         <v>500</v>
       </c>
       <c r="L3" s="12">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="M3" s="12">
         <v>15000</v>
@@ -10884,7 +10648,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="18">
-        <v>850000</v>
+        <v>900000</v>
       </c>
       <c r="D4" s="33">
         <v>0.2</v>
@@ -10905,7 +10669,7 @@
         <v>50</v>
       </c>
       <c r="K4" s="12">
-        <v>1000</v>
+        <v>1700</v>
       </c>
       <c r="M4"/>
     </row>
@@ -10940,7 +10704,7 @@
         <v>3</v>
       </c>
       <c r="K5" s="26">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="M5"/>
       <c r="N5" s="28"/>
@@ -10980,7 +10744,7 @@
         <v>3</v>
       </c>
       <c r="K7" s="26">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="M7"/>
       <c r="N7" s="28"/>
@@ -11027,7 +10791,7 @@
         <v>44</v>
       </c>
       <c r="J10" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -11082,4 +10846,214 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF624D77-2870-4555-B62D-733EBDFE0F64}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:Z16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11" customWidth="1"/>
+    <col min="5" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I1"/>
+      <c r="M1"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="I2"/>
+      <c r="M2"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="12">
+        <v>2200</v>
+      </c>
+      <c r="I3"/>
+      <c r="M3"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="18">
+        <v>75</v>
+      </c>
+      <c r="D4" s="41">
+        <v>50</v>
+      </c>
+      <c r="E4" s="41">
+        <v>25</v>
+      </c>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+    </row>
+    <row r="5" spans="1:26" s="70" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="70" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="70" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="12">
+        <v>25</v>
+      </c>
+      <c r="D6" s="12">
+        <v>50</v>
+      </c>
+      <c r="E6" s="12">
+        <v>100</v>
+      </c>
+      <c r="I6"/>
+      <c r="M6"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="12">
+        <v>20</v>
+      </c>
+      <c r="I7"/>
+      <c r="M7"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I8"/>
+      <c r="M8"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="12">
+        <v>150</v>
+      </c>
+      <c r="I9"/>
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="12">
+        <v>20</v>
+      </c>
+      <c r="I10"/>
+      <c r="M10"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="12">
+        <v>40</v>
+      </c>
+      <c r="I11"/>
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="39"/>
+      <c r="I12"/>
+      <c r="M12"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A13" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="I13"/>
+      <c r="M13"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I14"/>
+      <c r="M14"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I15"/>
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I16"/>
+      <c r="M16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixes to hsa and college expense
</commit_message>
<xml_diff>
--- a/python/Inputs/Inputs.xlsx
+++ b/python/Inputs/Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rthor\Dropbox\PC\Desktop\Projects\personalFinances\python\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E4CF37-82D5-48B0-89C3-957D1C961B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3DFD49-7FD4-4465-B87F-A6258CFBC055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="786" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="168">
   <si>
     <t>Years</t>
   </si>
@@ -521,9 +521,6 @@
     <t>Premium</t>
   </si>
   <si>
-    <t>HSA Deposit</t>
-  </si>
-  <si>
     <t>Chase</t>
   </si>
   <si>
@@ -552,6 +549,15 @@
   </si>
   <si>
     <t>IND-2</t>
+  </si>
+  <si>
+    <t>Traditional 401k</t>
+  </si>
+  <si>
+    <t>Roth 401k</t>
+  </si>
+  <si>
+    <t>Match 401k</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1176,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1371,6 +1377,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="20" fillId="35" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="34" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1741,7 +1750,7 @@
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:M106"/>
+  <dimension ref="A1:M110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -2028,68 +2037,96 @@
         <v>42</v>
       </c>
       <c r="C21" s="4">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="D21" s="4">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="E21" s="4">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="22" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="4">
+        <v>165</v>
+      </c>
+      <c r="B23" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.13</v>
+      </c>
+      <c r="D23" s="76">
+        <v>0.13</v>
+      </c>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B24" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="7">
         <v>0</v>
       </c>
-      <c r="D23" s="54">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B24" s="48"/>
-      <c r="C24" s="4">
+      <c r="D24" s="76">
         <v>0</v>
-      </c>
-      <c r="D24" s="54">
-        <v>2.3E-2</v>
       </c>
       <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B25" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="D25" s="76">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="48"/>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="54">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="48"/>
+      <c r="C28" s="4">
+        <v>0</v>
+      </c>
+      <c r="D28" s="54">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B29" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C29" s="4">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-    </row>
-    <row r="27" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-    </row>
-    <row r="28" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-    </row>
-    <row r="29" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="20"/>
@@ -2359,45 +2396,67 @@
       <c r="C96" s="20"/>
       <c r="D96" s="20"/>
     </row>
-    <row r="97" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C97" s="20"/>
       <c r="D97" s="20"/>
     </row>
-    <row r="98" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C98" s="20"/>
       <c r="D98" s="20"/>
     </row>
-    <row r="99" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C99" s="20"/>
       <c r="D99" s="20"/>
     </row>
-    <row r="100" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C100" s="20"/>
       <c r="D100" s="20"/>
     </row>
-    <row r="101" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C101" s="20"/>
       <c r="D101" s="20"/>
     </row>
-    <row r="102" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C102" s="20"/>
       <c r="D102" s="20"/>
     </row>
-    <row r="103" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C103" s="20"/>
       <c r="D103" s="20"/>
     </row>
-    <row r="104" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C104" s="20"/>
       <c r="D104" s="20"/>
     </row>
-    <row r="105" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C105" s="20"/>
       <c r="D105" s="20"/>
     </row>
-    <row r="106" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C106" s="20"/>
       <c r="D106" s="20"/>
+    </row>
+    <row r="107" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C107" s="20"/>
+      <c r="D107" s="20"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108"/>
+      <c r="B108"/>
+      <c r="C108" s="20"/>
+      <c r="D108" s="20"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109"/>
+      <c r="B109"/>
+      <c r="C109" s="20"/>
+      <c r="D109" s="20"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110"/>
+      <c r="B110"/>
+      <c r="C110" s="20"/>
+      <c r="D110" s="20"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2492,7 +2551,7 @@
       </c>
       <c r="B3" s="19">
         <f ca="1">A3+RANDBETWEEN(5,9)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="18">
         <v>23500</v>
@@ -2531,7 +2590,7 @@
       </c>
       <c r="B4" s="19">
         <f t="shared" ref="B4:B13" ca="1" si="0">A4+RANDBETWEEN(5,9)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" s="18">
         <v>32000</v>
@@ -2562,11 +2621,11 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="17">
         <f ca="1">IF(B3&lt;Inputs!$C$3,B3,"")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B5" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="18">
         <v>30000</v>
@@ -2600,11 +2659,11 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
         <f ca="1">IF(B4&lt;Inputs!$C$3,B4,"")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="18">
         <v>30000</v>
@@ -2629,11 +2688,11 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <f ca="1">IF(B5&lt;Inputs!$C$3,B5,"")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="18">
         <v>35000</v>
@@ -2664,7 +2723,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <f ca="1">IF(B6&lt;Inputs!$C$3,B6,"")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="19">
         <f t="shared" ca="1" si="0"/>
@@ -2693,11 +2752,11 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <f ca="1">IF(B7&lt;Inputs!$C$3,B7,"")</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C9" s="18">
         <v>40000</v>
@@ -2751,15 +2810,15 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
         <f ca="1">IF(B9&lt;Inputs!$C$3,B9,"")</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B11" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C11" s="18">
         <f ca="1">IF(ISNUMBER(B11),RANDBETWEEN(40000,60000),"")</f>
-        <v>48978</v>
+        <v>55417</v>
       </c>
       <c r="D11" s="33">
         <f t="shared" ca="1" si="1"/>
@@ -2785,11 +2844,11 @@
       </c>
       <c r="B12" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" s="18">
         <f t="shared" ref="C12:C19" ca="1" si="5">IF(ISNUMBER(B12),RANDBETWEEN(40000,60000),"")</f>
-        <v>57637</v>
+        <v>47242</v>
       </c>
       <c r="D12" s="33">
         <f t="shared" ca="1" si="1"/>
@@ -2811,15 +2870,15 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <f ca="1">IF(B11&lt;Inputs!$C$3,B11,"")</f>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B13" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C13" s="18">
         <f t="shared" ca="1" si="5"/>
-        <v>50463</v>
+        <v>46528</v>
       </c>
       <c r="D13" s="33">
         <f t="shared" ca="1" si="1"/>
@@ -2841,15 +2900,15 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <f ca="1">IF(B12&lt;Inputs!$C$3,B12,"")</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" s="19">
         <f t="shared" ref="B14:B19" ca="1" si="6">IF(ISNUMBER(A14),A14+RANDBETWEEN(5,9),"")</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" s="18">
         <f t="shared" ca="1" si="5"/>
-        <v>42871</v>
+        <v>58442</v>
       </c>
       <c r="D14" s="33">
         <f t="shared" ca="1" si="1"/>
@@ -2869,33 +2928,33 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="17">
+      <c r="A15" s="17" t="str">
         <f ca="1">IF(B13&lt;Inputs!$C$3,B13,"")</f>
-        <v>39</v>
-      </c>
-      <c r="B15" s="19">
+        <v/>
+      </c>
+      <c r="B15" s="19" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>47</v>
-      </c>
-      <c r="C15" s="18">
+        <v/>
+      </c>
+      <c r="C15" s="18" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>58428</v>
-      </c>
-      <c r="D15" s="33">
+        <v/>
+      </c>
+      <c r="D15" s="33" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="E15" s="33">
+        <v/>
+      </c>
+      <c r="E15" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.15</v>
-      </c>
-      <c r="F15" s="60">
+        <v/>
+      </c>
+      <c r="F15" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="G15" s="37">
+        <v/>
+      </c>
+      <c r="G15" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9E-2</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -5014,7 +5073,7 @@
         <v>57</v>
       </c>
       <c r="D9" s="43" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E9" s="43"/>
     </row>
@@ -5716,10 +5775,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A2:M14"/>
+  <dimension ref="A2:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5850,32 +5909,21 @@
       <c r="C11" s="44" t="b">
         <v>1</v>
       </c>
+      <c r="D11" s="45"/>
       <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B12" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="12">
-        <v>0</v>
-      </c>
+      <c r="A12" s="30"/>
       <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="30"/>
+      <c r="A13" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>119</v>
+      </c>
       <c r="E13" s="28"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="E14" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6564,7 +6612,7 @@
   <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6699,7 +6747,7 @@
       </c>
       <c r="B13" s="64">
         <f ca="1">(1+(RANDBETWEEN(2,10)/100))*B12</f>
-        <v>436000.00000000006</v>
+        <v>424000</v>
       </c>
       <c r="C13" s="64"/>
     </row>
@@ -6710,7 +6758,7 @@
       </c>
       <c r="B14" s="64">
         <f t="shared" ref="B14:B26" ca="1" si="1">(1+(RANDBETWEEN(2,10)/100))*B13</f>
-        <v>457800.00000000006</v>
+        <v>432480</v>
       </c>
       <c r="C14" s="64"/>
     </row>
@@ -6721,7 +6769,7 @@
       </c>
       <c r="B15" s="64">
         <f t="shared" ca="1" si="1"/>
-        <v>480690.00000000006</v>
+        <v>471403.2</v>
       </c>
       <c r="C15" s="64"/>
     </row>
@@ -6732,7 +6780,7 @@
       </c>
       <c r="B16" s="64">
         <f t="shared" ca="1" si="1"/>
-        <v>528759.00000000012</v>
+        <v>490259.32800000004</v>
       </c>
       <c r="C16" s="64"/>
     </row>
@@ -6743,7 +6791,7 @@
       </c>
       <c r="B17" s="64">
         <f t="shared" ca="1" si="1"/>
-        <v>565772.13000000012</v>
+        <v>504967.10784000007</v>
       </c>
       <c r="C17" s="64"/>
     </row>
@@ -6754,7 +6802,7 @@
       </c>
       <c r="B18" s="64">
         <f t="shared" ca="1" si="1"/>
-        <v>605376.17910000018</v>
+        <v>555463.81862400007</v>
       </c>
       <c r="C18" s="64"/>
     </row>
@@ -6765,7 +6813,7 @@
       </c>
       <c r="B19" s="64">
         <f t="shared" ca="1" si="1"/>
-        <v>653806.27342800028</v>
+        <v>611010.20048640016</v>
       </c>
       <c r="C19" s="64"/>
     </row>
@@ -6776,7 +6824,7 @@
       </c>
       <c r="B20" s="64">
         <f t="shared" ca="1" si="1"/>
-        <v>666882.39889656031</v>
+        <v>635450.60850585625</v>
       </c>
       <c r="C20" s="64"/>
     </row>
@@ -6787,7 +6835,7 @@
       </c>
       <c r="B21" s="64">
         <f t="shared" ca="1" si="1"/>
-        <v>686888.87086345709</v>
+        <v>692641.16327138338</v>
       </c>
       <c r="C21" s="64"/>
     </row>
@@ -6798,7 +6846,7 @@
       </c>
       <c r="B22" s="64">
         <f t="shared" ca="1" si="1"/>
-        <v>721233.31440663</v>
+        <v>720346.80980223871</v>
       </c>
       <c r="C22" s="64"/>
     </row>
@@ -6809,7 +6857,7 @@
       </c>
       <c r="B23" s="64">
         <f t="shared" ca="1" si="1"/>
-        <v>757294.98012696148</v>
+        <v>749160.68219432828</v>
       </c>
       <c r="C23" s="64"/>
     </row>
@@ -6820,7 +6868,7 @@
       </c>
       <c r="B24" s="64">
         <f t="shared" ca="1" si="1"/>
-        <v>817878.5785371185</v>
+        <v>824076.75041376112</v>
       </c>
       <c r="C24" s="64"/>
     </row>
@@ -6831,7 +6879,7 @@
       </c>
       <c r="B25" s="64">
         <f t="shared" ca="1" si="1"/>
-        <v>899666.43639083044</v>
+        <v>906484.42545513727</v>
       </c>
       <c r="C25" s="64"/>
     </row>
@@ -6842,7 +6890,7 @@
       </c>
       <c r="B26" s="64">
         <f t="shared" ca="1" si="1"/>
-        <v>953646.4225742803</v>
+        <v>951808.6467278942</v>
       </c>
       <c r="C26" s="64"/>
     </row>
@@ -7516,7 +7564,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C1" s="5"/>
     </row>
@@ -8062,7 +8110,7 @@
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8078,7 +8126,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="77" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="13" t="s">
@@ -8088,12 +8136,12 @@
       <c r="D1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="76"/>
+      <c r="A2" s="77"/>
       <c r="B2" s="21" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>27</v>
@@ -8125,7 +8173,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F3" s="73"/>
       <c r="G3" s="41"/>
@@ -8240,14 +8288,14 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B8" s="25">
         <f>130000-B9</f>
         <v>85000</v>
       </c>
       <c r="C8" s="65" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>31</v>
@@ -8261,13 +8309,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B9" s="25">
         <v>45000</v>
       </c>
       <c r="C9" s="65" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>30</v>
@@ -8281,13 +8329,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B10" s="25">
         <v>75000</v>
       </c>
       <c r="C10" s="65" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>31</v>
@@ -8301,13 +8349,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B11" s="25">
         <v>15000</v>
       </c>
       <c r="C11" s="65" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>30</v>
@@ -8922,7 +8970,7 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView zoomScale="84" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9161,19 +9209,19 @@
         <v>savings</v>
       </c>
       <c r="B12" s="22">
-        <v>250</v>
+        <v>10</v>
       </c>
       <c r="C12" s="22">
-        <v>275</v>
+        <v>10</v>
       </c>
       <c r="D12" s="36">
-        <v>250</v>
+        <v>10</v>
       </c>
       <c r="E12" s="36">
-        <v>175</v>
+        <v>10</v>
       </c>
       <c r="F12" s="36">
-        <v>125</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.3">
@@ -9629,7 +9677,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9640,7 +9688,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="77" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="13" t="s">
@@ -9651,7 +9699,7 @@
       <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="76"/>
+      <c r="A2" s="77"/>
       <c r="B2" s="21" t="s">
         <v>16</v>
       </c>
@@ -9831,7 +9879,7 @@
         <v>savings</v>
       </c>
       <c r="B13" s="23">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C13" s="23">
         <v>0.01</v>
@@ -10855,7 +10903,7 @@
   </sheetPr>
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>